<commit_message>
Update excel tai san cong
</commit_message>
<xml_diff>
--- a/CSDLGia_ASP/wwwroot/UpLoad/File/DinhGia/Excel/FileExcelGiaThueTaiNguyen.xlsx
+++ b/CSDLGia_ASP/wwwroot/UpLoad/File/DinhGia/Excel/FileExcelGiaThueTaiNguyen.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CSDLGia_ASP\CSDLGia_ASP\wwwroot\UpLoad\File\DinhGia\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4961B95-47C2-4F3F-8E9C-15AB7574F86B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C68EB1D8-566A-4106-95D9-8618DDDA07B4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="11310" xr2:uid="{6AF4210B-D7D1-451E-A048-5B80F2CEA5CC}"/>
+    <workbookView xWindow="1725" yWindow="5100" windowWidth="21420" windowHeight="10725" xr2:uid="{6AF4210B-D7D1-451E-A048-5B80F2CEA5CC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="10">
   <si>
     <t>Phân loại</t>
   </si>
@@ -54,10 +54,7 @@
     <t>Tên nhóm</t>
   </si>
   <si>
-    <t>Nhà 1 tầng, tường 111</t>
-  </si>
-  <si>
-    <t>Nhà 1 tầng, tường 200</t>
+    <t>Giá Thuế Tài Nguyên Khoảng sản kim loại</t>
   </si>
 </sst>
 </file>
@@ -436,13 +433,13 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="25.28515625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="24.5703125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="60" style="1" customWidth="1"/>
     <col min="3" max="3" width="24.5703125" customWidth="1"/>
     <col min="4" max="4" width="25.7109375" customWidth="1"/>
     <col min="5" max="5" width="38.42578125" customWidth="1"/>
@@ -507,7 +504,7 @@
         <v>231130224114</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>5</v>
@@ -524,7 +521,7 @@
         <v>231130224114</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>6</v>
@@ -541,7 +538,7 @@
         <v>231130224114</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>7</v>

</xml_diff>